<commit_message>
Table class is added; some changes to functions from other classes; extras are removed from food.xlsx
From food.xlsx extras are deleted.

In the Restaurant free_table function is added.

In the Order a new parameter 'preferences' (for NOs and EXTRAs) is added.
</commit_message>
<xml_diff>
--- a/food.xlsx
+++ b/food.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rener\Documents\GitHub\EPR_Teamwork\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86BCB51A-4D62-4969-9B73-EC9616E14776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61D3FFC2-2AB4-4EDA-B89F-148E21973B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{A92A5A5B-9D7A-4456-B8FB-237F386228F9}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="30">
   <si>
     <t>name</t>
   </si>
@@ -64,9 +64,6 @@
     <t>CHILI-BURGER</t>
   </si>
   <si>
-    <t>beef, hot</t>
-  </si>
-  <si>
     <t>PIZZA-MARGARITA</t>
   </si>
   <si>
@@ -113,24 +110,6 @@
   </si>
   <si>
     <t>alcohol</t>
-  </si>
-  <si>
-    <t>CHEESE</t>
-  </si>
-  <si>
-    <t>extras</t>
-  </si>
-  <si>
-    <t>PICKLES</t>
-  </si>
-  <si>
-    <t>TOMATOES</t>
-  </si>
-  <si>
-    <t>MEAT</t>
-  </si>
-  <si>
-    <t>FRIES</t>
   </si>
 </sst>
 </file>
@@ -614,8 +593,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -991,28 +973,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4496DC-765E-42C3-ABBC-8710D94917DC}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19.46484375" customWidth="1"/>
+    <col min="2" max="2" width="9.06640625" style="1"/>
+    <col min="3" max="3" width="14.19921875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1020,13 +1005,13 @@
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>12</v>
       </c>
     </row>
@@ -1034,13 +1019,13 @@
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>13</v>
       </c>
     </row>
@@ -1048,13 +1033,13 @@
       <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>9</v>
       </c>
     </row>
@@ -1062,13 +1047,13 @@
       <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>10</v>
       </c>
     </row>
@@ -1076,13 +1061,13 @@
       <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>12</v>
       </c>
     </row>
@@ -1090,252 +1075,182 @@
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1">
         <v>12.5</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>3.5</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s">
-        <v>21</v>
-      </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>2.5</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
-        <v>21</v>
-      </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B19" t="s">
-        <v>20</v>
-      </c>
-      <c r="C19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>32</v>
-      </c>
-      <c r="D20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" t="s">
-        <v>32</v>
-      </c>
-      <c r="D22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A23" t="s">
-        <v>35</v>
-      </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-      <c r="C24" t="s">
-        <v>32</v>
-      </c>
-      <c r="D24">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>